<commit_message>
upload materi 3 excel basic
</commit_message>
<xml_diff>
--- a/Materi Belajar Excel/Excel Latihan Praktek.xlsx
+++ b/Materi Belajar Excel/Excel Latihan Praktek.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,34 +24,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Daftar barang</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nama </t>
-  </si>
-  <si>
-    <t>Harga</t>
-  </si>
-  <si>
-    <t>Beras</t>
-  </si>
-  <si>
-    <t>Micin</t>
-  </si>
-  <si>
-    <t>Garam</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Stock Buah Toko Segar</t>
+  </si>
+  <si>
+    <t>Nama Buah</t>
+  </si>
+  <si>
+    <t>Stok Tersisa</t>
+  </si>
+  <si>
+    <t>Harga Satuan</t>
+  </si>
+  <si>
+    <t>Apel Jeruk</t>
+  </si>
+  <si>
+    <t>Jeruk</t>
+  </si>
+  <si>
+    <t>Anggur</t>
+  </si>
+  <si>
+    <t>Melon</t>
+  </si>
+  <si>
+    <t>Semangka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah Stok Tersedia </t>
+  </si>
+  <si>
+    <t>Rata-rata Stok per Buah</t>
+  </si>
+  <si>
+    <t>Banyaknya Jenis Buah</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average </t>
+  </si>
+  <si>
+    <t>count (angka)/counta(bisa angka/huruf)</t>
+  </si>
+  <si>
+    <t>Harga Paling Tinggi</t>
+  </si>
+  <si>
+    <t>Harga Paling Rendah</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,24 +104,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,19 +119,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,12 +151,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,66 +438,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f>SUM(B4:B7)</f>
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(B4,B6,B8)</f>
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f>COUNTA(B4:B5)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4">
-        <v>400</v>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <f>MAX(C4:C8)</f>
+        <v>20000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <f>MIN(C4:C8)</f>
+        <v>5000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
materi 4 & 5 selesai, lanjut excel midle
</commit_message>
<xml_diff>
--- a/Materi Belajar Excel/Excel Latihan Praktek.xlsx
+++ b/Materi Belajar Excel/Excel Latihan Praktek.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Stock Buah Toko Segar</t>
   </si>
@@ -81,6 +82,111 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>No. Pemesanan</t>
+  </si>
+  <si>
+    <t>Nama Customer</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>Domisili</t>
+  </si>
+  <si>
+    <t>Andi</t>
+  </si>
+  <si>
+    <t>Budi</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Dewi</t>
+  </si>
+  <si>
+    <t>Eko</t>
+  </si>
+  <si>
+    <t>Fiona</t>
+  </si>
+  <si>
+    <t>Gina</t>
+  </si>
+  <si>
+    <t>Hesti</t>
+  </si>
+  <si>
+    <t>Igna</t>
+  </si>
+  <si>
+    <t>Juned</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Merry</t>
+  </si>
+  <si>
+    <t>Nino</t>
+  </si>
+  <si>
+    <t>Osa</t>
+  </si>
+  <si>
+    <t>Laki-Laki</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Palembang</t>
+  </si>
+  <si>
+    <t>Sorong</t>
+  </si>
+  <si>
+    <t>Makassar</t>
+  </si>
+  <si>
+    <t>Pekanbaru</t>
+  </si>
+  <si>
+    <t>Tasikmalaya</t>
+  </si>
+  <si>
+    <t>Semarang</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Yogyakarta</t>
+  </si>
+  <si>
+    <t>Denpasar</t>
+  </si>
+  <si>
+    <t>Mataram</t>
+  </si>
+  <si>
+    <t>Pontianak</t>
+  </si>
+  <si>
+    <t>Ambon</t>
   </si>
 </sst>
 </file>
@@ -151,13 +257,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,6 +282,873 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stok Tersisa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Apel Jeruk</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jeruk</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Anggur</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Melon</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Semangka</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="396058704"/>
+        <c:axId val="396059488"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="396058704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396059488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="396059488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396058704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,5 +1562,251 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>104</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>105</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>106</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>111</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>112</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>113</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>114</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>115</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
materi 2 vlookup excel midle selesai
</commit_message>
<xml_diff>
--- a/Materi Belajar Excel/Excel Latihan Praktek.xlsx
+++ b/Materi Belajar Excel/Excel Latihan Praktek.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belajar Data Analyst\Bel4jar-menjadi-data-analist\Materi Belajar Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belajar Data Analyst\Materi Belajar Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>Stock Buah Toko Segar</t>
   </si>
@@ -458,11 +458,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="253243160"/>
-        <c:axId val="253243544"/>
+        <c:axId val="380540432"/>
+        <c:axId val="380542872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253243160"/>
+        <c:axId val="380540432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253243544"/>
+        <c:crossAx val="380542872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -513,7 +513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253243544"/>
+        <c:axId val="380542872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253243160"/>
+        <c:crossAx val="380540432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2101,7 +2101,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,6 +2141,10 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2">
+        <f>IFERROR(VLOOKUP(E2,A1:$C$6,3,0),"No Data")</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2155,6 +2159,10 @@
       <c r="E3" t="s">
         <v>62</v>
       </c>
+      <c r="F3" t="str">
+        <f>IFERROR(VLOOKUP(E3,A2:$C$6,3,0),"No Data")</f>
+        <v>No Data</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2169,6 +2177,10 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
+      <c r="F4">
+        <f>IFERROR(VLOOKUP(E4,A3:$C$6,3,0),"No Data")</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2178,6 +2190,13 @@
         <v>12000</v>
       </c>
       <c r="C5" s="1">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(VLOOKUP(E5,A4:$C$6,3,0),"No Data")</f>
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
materi 3 midle sudah selesai
</commit_message>
<xml_diff>
--- a/Materi Belajar Excel/Excel Latihan Praktek.xlsx
+++ b/Materi Belajar Excel/Excel Latihan Praktek.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>Stock Buah Toko Segar</t>
   </si>
@@ -216,6 +217,30 @@
   </si>
   <si>
     <t>Lychee</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir</t>
+  </si>
+  <si>
+    <t>Umur</t>
+  </si>
+  <si>
+    <t>Ruben Ardi</t>
+  </si>
+  <si>
+    <t>Disti Liana</t>
+  </si>
+  <si>
+    <t>Juned Abdullah</t>
+  </si>
+  <si>
+    <t>Aryanne Marina</t>
+  </si>
+  <si>
+    <t>Mega Sarita</t>
   </si>
 </sst>
 </file>
@@ -245,7 +270,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +339,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,11 +495,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="380540432"/>
-        <c:axId val="380542872"/>
+        <c:axId val="386666952"/>
+        <c:axId val="386667344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="380540432"/>
+        <c:axId val="386666952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380542872"/>
+        <c:crossAx val="386667344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -513,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="380542872"/>
+        <c:axId val="386667344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380540432"/>
+        <c:crossAx val="386666952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2100,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
@@ -2214,4 +2251,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="10">
+        <v>37987</v>
+      </c>
+      <c r="C2" s="1">
+        <f ca="1">DATEDIF(B2,TODAY(),"m")</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="10">
+        <v>39858</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C7" ca="1" si="0">DATEDIF(B3,TODAY(),"m")</f>
+        <v>171</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="10">
+        <v>33835</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42155</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10">
+        <v>35885</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>44474</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
materi 4 midle belum selesai
</commit_message>
<xml_diff>
--- a/Materi Belajar Excel/Excel Latihan Praktek.xlsx
+++ b/Materi Belajar Excel/Excel Latihan Praktek.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Stock Buah Toko Segar</t>
   </si>
@@ -241,6 +242,18 @@
   </si>
   <si>
     <t>Mega Sarita</t>
+  </si>
+  <si>
+    <t>Tanggal Awal</t>
+  </si>
+  <si>
+    <t>Tanggal Akhir</t>
+  </si>
+  <si>
+    <t>Hari Kerja</t>
+  </si>
+  <si>
+    <t>Tanggal Merah &amp; Cuti</t>
   </si>
 </sst>
 </file>
@@ -270,7 +283,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,6 +364,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,11 +517,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="386666952"/>
-        <c:axId val="386667344"/>
+        <c:axId val="381807672"/>
+        <c:axId val="381809632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="386666952"/>
+        <c:axId val="381807672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386667344"/>
+        <c:crossAx val="381809632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="386667344"/>
+        <c:axId val="381809632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386666952"/>
+        <c:crossAx val="381807672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2257,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -2355,4 +2377,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44227</v>
+      </c>
+      <c r="B2" s="10">
+        <v>44255</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>44243</v>
+      </c>
+      <c r="B3" s="10">
+        <v>44255</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>